<commit_message>
Update CDM-2 and CDP
Correção do campo "Indice de Custo" no CDM-2 onde faltava o símbolo %.
Atualizado o CDP com a remoção da coluna "Taxa de Conclusão". Essas
pequenas correções foram realizadas pela atividade de rotina "Conduzir
Projeto".
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDM-2.xlsx
+++ b/Projeto/GPR/PG2016-1-CDM-2.xlsx
@@ -112,9 +112,6 @@
     <t>AT11</t>
   </si>
   <si>
-    <t>Índice de Custo</t>
-  </si>
-  <si>
     <t>PG2016-1 - Checklist de Monitoramento (CDM) - 2</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Observações:</t>
+  </si>
+  <si>
+    <t>Índice de Custo (%)</t>
   </si>
 </sst>
 </file>
@@ -314,8 +314,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,11 +377,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -371,32 +395,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -734,75 +734,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25">
-      <c r="A1" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="A1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="16">
+      <c r="B3" s="15"/>
+      <c r="C3" s="24">
         <v>42660</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="42.75">
       <c r="A6" s="2" t="s">
@@ -814,19 +814,19 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -839,14 +839,14 @@
       <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="8">
         <v>5180</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="26">
+      <c r="E7" s="9"/>
+      <c r="F7" s="8">
         <v>5180</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="5">
         <f>((C7)/B7)-1</f>
         <v>0</v>
@@ -866,14 +866,14 @@
       <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="8">
         <v>260</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="26">
+      <c r="E8" s="9"/>
+      <c r="F8" s="8">
         <v>170</v>
       </c>
-      <c r="G8" s="27"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="5">
         <f>((C8)/B8)-1</f>
         <v>-0.33333333333333337</v>
@@ -893,14 +893,14 @@
       <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="8">
         <v>100</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="26">
+      <c r="E9" s="9"/>
+      <c r="F9" s="8">
         <v>100</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="5">
         <f>((C9)/B9)-1</f>
         <v>0</v>
@@ -920,14 +920,14 @@
       <c r="C10" s="4">
         <v>8</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="8">
         <v>380</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="26">
+      <c r="E10" s="9"/>
+      <c r="F10" s="8">
         <v>380</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="5">
         <f>((C10)/B10)-1</f>
         <v>0</v>
@@ -939,15 +939,15 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="7">
         <f>SUM(H7:H10)</f>
         <v>-0.33333333333333337</v>
@@ -958,15 +958,15 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="5">
         <f>AVERAGE(H7:H10)</f>
         <v>-8.3333333333333343E-2</v>
@@ -977,131 +977,118 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" ht="18">
+      <c r="A16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" ht="18">
-      <c r="A16" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="8"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="A19:I21"/>
@@ -1118,6 +1105,19 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A12:G12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1135,15 +1135,15 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">

</xml_diff>